<commit_message>
update test excel burundi
</commit_message>
<xml_diff>
--- a/Design/Burundi final test.xlsx
+++ b/Design/Burundi final test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabrina\Documents\GitHub\IRP-framework\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACB2DE0-0439-4F3D-9934-E7EAA14C3F49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131E917F-5C68-41A6-8A50-852865A06A45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{5975349C-58A3-4B5B-8FE6-1441333428CB}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{5975349C-58A3-4B5B-8FE6-1441333428CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Schools" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Name_ID</t>
   </si>
@@ -149,9 +149,6 @@
     <t>BIGWA I</t>
   </si>
   <si>
-    <t>BIGWA II</t>
-  </si>
-  <si>
     <t>BIKINGI</t>
   </si>
   <si>
@@ -186,6 +183,30 @@
   </si>
   <si>
     <t>Storage Cost</t>
+  </si>
+  <si>
+    <t>MUTUMBA II</t>
+  </si>
+  <si>
+    <t>MUYANGE I</t>
+  </si>
+  <si>
+    <t>MUYANGE II</t>
+  </si>
+  <si>
+    <t>MUYUGA</t>
+  </si>
+  <si>
+    <t>MUZIMA</t>
+  </si>
+  <si>
+    <t>MWAZA</t>
+  </si>
+  <si>
+    <t>MWUMBA</t>
+  </si>
+  <si>
+    <t>NDAGO</t>
   </si>
 </sst>
 </file>
@@ -607,8 +628,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0AFBE7F-EE6B-43D3-AC29-0F1EA5EDD28B}" name="Tabelle1" displayName="Tabelle1" ref="A1:K9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:K9" xr:uid="{92D50160-D1EB-4CE0-BC5E-AD10E29A0DA1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0AFBE7F-EE6B-43D3-AC29-0F1EA5EDD28B}" name="Tabelle1" displayName="Tabelle1" ref="A1:K16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:K16" xr:uid="{92D50160-D1EB-4CE0-BC5E-AD10E29A0DA1}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{E5C5CD31-DB14-4BCA-9F11-3AA7A7551D2B}" name="Name_ID" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{EB335BE7-11E3-434A-B317-30C0F850D50E}" name="Total Sum of Beneficiaries" dataDxfId="18"/>
@@ -939,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65252ADD-2539-421B-8440-8530B4AE7D99}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -978,16 +999,16 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -1100,31 +1121,31 @@
         <v>11</v>
       </c>
       <c r="B5" s="1">
-        <v>646</v>
+        <v>866</v>
       </c>
       <c r="C5" s="1">
-        <v>1.9670699999999999</v>
+        <v>2.5950000000000002</v>
       </c>
       <c r="D5" s="1">
-        <v>0.12920000000000001</v>
+        <v>0.17320000000000002</v>
       </c>
       <c r="E5" s="1">
-        <v>0.64600000000000002</v>
+        <v>0.8660000000000001</v>
       </c>
       <c r="F5" s="1">
-        <v>-3.4071859999999998</v>
+        <v>-3.5404490000000002</v>
       </c>
       <c r="G5" s="1">
-        <v>29.390370000000001</v>
+        <v>29.852342</v>
       </c>
       <c r="H5" s="1">
-        <v>3.19</v>
+        <v>3.84</v>
       </c>
       <c r="I5" s="1">
-        <v>0.65</v>
+        <v>0.87</v>
       </c>
       <c r="J5" s="1">
-        <v>0.87</v>
+        <v>1.97</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -1132,34 +1153,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1">
-        <v>866</v>
+        <v>635</v>
       </c>
       <c r="C6" s="1">
-        <v>2.5950000000000002</v>
+        <v>1.933575</v>
       </c>
       <c r="D6" s="1">
-        <v>0.17320000000000002</v>
+        <v>0.127</v>
       </c>
       <c r="E6" s="1">
-        <v>0.8660000000000001</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="F6" s="1">
-        <v>-3.5404490000000002</v>
+        <v>-3.5886499999999999</v>
       </c>
       <c r="G6" s="1">
-        <v>29.852342</v>
+        <v>29.35942</v>
       </c>
       <c r="H6" s="1">
-        <v>3.84</v>
+        <v>3.81</v>
       </c>
       <c r="I6" s="1">
-        <v>0.87</v>
+        <v>0.64</v>
       </c>
       <c r="J6" s="1">
-        <v>1.97</v>
+        <v>1.76</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -1167,34 +1188,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1">
-        <v>1160</v>
+        <v>1168</v>
       </c>
       <c r="C7" s="1">
-        <v>1.74</v>
+        <v>4.8400000000000007</v>
       </c>
       <c r="D7" s="1">
-        <v>0.23200000000000001</v>
+        <v>0.23360000000000003</v>
       </c>
       <c r="E7" s="1">
-        <v>1.1600000000000001</v>
+        <v>1.1680000000000001</v>
       </c>
       <c r="F7" s="1">
-        <v>-3.4605839999999999</v>
+        <v>-2.8280959999999999</v>
       </c>
       <c r="G7" s="1">
-        <v>29.491987000000002</v>
+        <v>30.127786</v>
       </c>
       <c r="H7" s="1">
-        <v>6.49</v>
+        <v>6.73</v>
       </c>
       <c r="I7" s="1">
-        <v>1.1599999999999999</v>
+        <v>1.17</v>
       </c>
       <c r="J7" s="1">
-        <v>1.22</v>
+        <v>1.7</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
@@ -1202,34 +1223,34 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
-        <v>548</v>
+        <v>590</v>
       </c>
       <c r="C8" s="1">
-        <v>1.66866</v>
+        <v>1.843</v>
       </c>
       <c r="D8" s="1">
-        <v>0.10960000000000002</v>
+        <v>0.11800000000000001</v>
       </c>
       <c r="E8" s="1">
-        <v>0.54800000000000004</v>
+        <v>0.59000000000000008</v>
       </c>
       <c r="F8" s="1">
-        <v>-3.703722</v>
+        <v>-3.1234920000000002</v>
       </c>
       <c r="G8" s="1">
-        <v>29.918804000000002</v>
+        <v>29.34451</v>
       </c>
       <c r="H8" s="1">
-        <v>2.48</v>
+        <v>2.46</v>
       </c>
       <c r="I8" s="1">
-        <v>0.55000000000000004</v>
+        <v>0.59</v>
       </c>
       <c r="J8" s="1">
-        <v>0.69</v>
+        <v>1.33</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -1237,36 +1258,281 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
+        <v>847</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.2709999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.16940000000000002</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.84700000000000009</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-3.7038009999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>29.834140999999999</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.83</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1">
+        <v>848</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.7759999999999998</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.16960000000000003</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.84800000000000009</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-3.5700080000000001</v>
+      </c>
+      <c r="G10" s="1">
+        <v>29.841771999999999</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4.47</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1">
+        <v>708</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.1558600000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.1416</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-3.5510470000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>29.378411</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3.05</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.28</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1">
+        <v>903</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3.6209999999999996</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.18060000000000004</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.90300000000000025</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-3.2078739999999999</v>
+      </c>
+      <c r="G12" s="1">
+        <v>29.872033999999999</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.39</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1">
+        <v>635</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.127</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-3.8171219999999999</v>
+      </c>
+      <c r="G13" s="1">
+        <v>29.923649000000001</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3.47</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1160</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1.1600000000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-3.4605839999999999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>29.491987000000002</v>
+      </c>
+      <c r="H14" s="1">
+        <v>6.49</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>548</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.66866</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.10960000000000002</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-3.703722</v>
+      </c>
+      <c r="G15" s="1">
+        <v>29.918804000000002</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2.48</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
         <v>551</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C16" s="1">
         <v>0.82699999999999996</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D16" s="1">
         <v>0.11020000000000001</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E16" s="1">
         <v>0.55100000000000005</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F16" s="1">
         <v>-3.7073900000000002</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G16" s="1">
         <v>29.866121</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H16" s="1">
         <v>2.86</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I16" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J16" s="1">
         <v>0.92</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K16" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1284,7 +1550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5307C4E-D51E-4E16-960B-CB790613AD8F}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1305,21 +1571,21 @@
         <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>-3.36</v>
@@ -1342,7 +1608,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>-2.911</v>
@@ -1365,7 +1631,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>-3.4279999999999999</v>

</xml_diff>

<commit_message>
included different types of vehicles in GUI and ISI
</commit_message>
<xml_diff>
--- a/Design/Burundi final test.xlsx
+++ b/Design/Burundi final test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabrina\Documents\GitHub\IRP-framework\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131E917F-5C68-41A6-8A50-852865A06A45}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298195EB-8241-4D60-9593-668247536485}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{5975349C-58A3-4B5B-8FE6-1441333428CB}"/>
+    <workbookView xWindow="3292" yWindow="1020" windowWidth="15428" windowHeight="11760" activeTab="2" xr2:uid="{5975349C-58A3-4B5B-8FE6-1441333428CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Schools" sheetId="1" r:id="rId1"/>
     <sheet name="Warehouses" sheetId="2" r:id="rId2"/>
+    <sheet name="VehicleFleet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>Name_ID</t>
   </si>
@@ -207,6 +208,144 @@
   </si>
   <si>
     <t>NDAGO</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Plate Nr</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Capacity in MT</t>
+  </si>
+  <si>
+    <t>GITEGA</t>
+  </si>
+  <si>
+    <t>CD44A95</t>
+  </si>
+  <si>
+    <t>RENAULT 6X4</t>
+  </si>
+  <si>
+    <t>350,34</t>
+  </si>
+  <si>
+    <t>CD44B02</t>
+  </si>
+  <si>
+    <t>CD44A89</t>
+  </si>
+  <si>
+    <t>RENAULT4X4</t>
+  </si>
+  <si>
+    <t>300,19</t>
+  </si>
+  <si>
+    <t>CD44A91</t>
+  </si>
+  <si>
+    <t>RENAULT 4X4</t>
+  </si>
+  <si>
+    <t>CD44A98</t>
+  </si>
+  <si>
+    <t>CD44A54</t>
+  </si>
+  <si>
+    <t>TOYOTA DYNA</t>
+  </si>
+  <si>
+    <t>E059AIT</t>
+  </si>
+  <si>
+    <t>TOYOTA PIC-UP</t>
+  </si>
+  <si>
+    <t>Land cruiser</t>
+  </si>
+  <si>
+    <t>CD107-98U</t>
+  </si>
+  <si>
+    <t>TRAILER</t>
+  </si>
+  <si>
+    <t>BUJUMBURA</t>
+  </si>
+  <si>
+    <t>CD44A96</t>
+  </si>
+  <si>
+    <t>CD44A52</t>
+  </si>
+  <si>
+    <t>CD44A81</t>
+  </si>
+  <si>
+    <t>ISUZU</t>
+  </si>
+  <si>
+    <t>CD44A55</t>
+  </si>
+  <si>
+    <t>CD44A86</t>
+  </si>
+  <si>
+    <t>CD44A87</t>
+  </si>
+  <si>
+    <t>CD44A35</t>
+  </si>
+  <si>
+    <t>CD44A25</t>
+  </si>
+  <si>
+    <t>CD44A31</t>
+  </si>
+  <si>
+    <t>TOYOTA  PIC-UP</t>
+  </si>
+  <si>
+    <t>E058AIT</t>
+  </si>
+  <si>
+    <t>NGOZI</t>
+  </si>
+  <si>
+    <t>CD44A88</t>
+  </si>
+  <si>
+    <t>CD44A94</t>
+  </si>
+  <si>
+    <t>CD44B01</t>
+  </si>
+  <si>
+    <t>CD44A90</t>
+  </si>
+  <si>
+    <t>CD44A57</t>
+  </si>
+  <si>
+    <t>CD44A48</t>
+  </si>
+  <si>
+    <t>CD44A43</t>
+  </si>
+  <si>
+    <t>CD44A33</t>
+  </si>
+  <si>
+    <t>CD107-69U</t>
   </si>
 </sst>
 </file>
@@ -264,7 +403,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -272,21 +411,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="31">
     <dxf>
       <font>
         <strike val="0"/>
@@ -428,6 +613,245 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -628,20 +1052,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0AFBE7F-EE6B-43D3-AC29-0F1EA5EDD28B}" name="Tabelle1" displayName="Tabelle1" ref="A1:K16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0AFBE7F-EE6B-43D3-AC29-0F1EA5EDD28B}" name="Tabelle1" displayName="Tabelle1" ref="A1:K16" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:K16" xr:uid="{92D50160-D1EB-4CE0-BC5E-AD10E29A0DA1}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E5C5CD31-DB14-4BCA-9F11-3AA7A7551D2B}" name="Name_ID" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{EB335BE7-11E3-434A-B317-30C0F850D50E}" name="Total Sum of Beneficiaries" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{548C3917-F847-4593-A558-D428505FFBD5}" name="Total Sum of Commodities" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{FE888112-53D5-4BA1-A73D-44D889EF4C4D}" name="Consumption per day in mt" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{16626E44-7904-4057-88C7-E83A60A6E39B}" name="Consumption per week in mt" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{BCB38217-DC5E-4A6B-90D0-4ED4225CA0CB}" name="Latitude" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{26DFB5ED-C9CB-4B62-A8A1-67C23CE6A976}" name="Longitude" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{AAB748E8-3709-4A83-AC4C-F11F31AEC3F8}" name="Capacity" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{8C005587-5BD7-4A0F-A7C5-F8E1AD8666E0}" name="Lower" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{6E875271-034D-4F07-BB60-56AAB571D1F0}" name="Initial" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{D05CCBD5-F14E-46D5-BC67-17C58FC0BB3E}" name="Storage Cost" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{E5C5CD31-DB14-4BCA-9F11-3AA7A7551D2B}" name="Name_ID" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{EB335BE7-11E3-434A-B317-30C0F850D50E}" name="Total Sum of Beneficiaries" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{548C3917-F847-4593-A558-D428505FFBD5}" name="Total Sum of Commodities" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{FE888112-53D5-4BA1-A73D-44D889EF4C4D}" name="Consumption per day in mt" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{16626E44-7904-4057-88C7-E83A60A6E39B}" name="Consumption per week in mt" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{BCB38217-DC5E-4A6B-90D0-4ED4225CA0CB}" name="Latitude" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{26DFB5ED-C9CB-4B62-A8A1-67C23CE6A976}" name="Longitude" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{AAB748E8-3709-4A83-AC4C-F11F31AEC3F8}" name="Capacity" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{8C005587-5BD7-4A0F-A7C5-F8E1AD8666E0}" name="Lower" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{6E875271-034D-4F07-BB60-56AAB571D1F0}" name="Initial" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{D05CCBD5-F14E-46D5-BC67-17C58FC0BB3E}" name="Storage Cost" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,6 +1084,20 @@
     <tableColumn id="8" xr3:uid="{F795114F-5871-4C9B-A276-526B58F4F0AC}" name="Fixed Cost" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C88B342E-860D-4CF9-9409-9BF05B92DC07}" name="Tabelle35" displayName="Tabelle35" ref="A1:E28" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
+  <autoFilter ref="A1:E28" xr:uid="{140EAF9C-EBEB-4D6E-AEE7-0C012A648023}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{08A0981D-418C-4F7D-91CF-9CE660861A78}" name="Warehouse" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{C734B396-0019-4F10-9D39-4B9C17A0C025}" name="Plate Nr" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{B2ECE29D-B197-48F8-ACC0-D09288F3CD21}" name="Make" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{9A05CAC1-95C8-4D47-8F85-9866F7615220}" name="Model" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{2110263D-43E8-4495-99BB-86FD4A69533A}" name="Capacity in MT" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -962,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65252ADD-2539-421B-8440-8530B4AE7D99}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1658,4 +2096,498 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67700975-B69D-4F23-A553-6F8EE09FC47B}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>